<commit_message>
Updated pass percentage to 3 decimal points
</commit_message>
<xml_diff>
--- a/uploads/year.xlsx
+++ b/uploads/year.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64844a5a8d2d907e/Desktop/Student Result Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayas\Desktop\Student Result Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{6F2B410E-521C-4E1B-99BE-C277D1D6B233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -847,8 +846,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -859,22 +858,33 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -929,35 +939,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,11 +1187,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1199,10 +1210,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>